<commit_message>
back to aws for keras testing
</commit_message>
<xml_diff>
--- a/data/orgs/about/about_model_training_results.xlsx
+++ b/data/orgs/about/about_model_training_results.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="25">
   <si>
     <t>Name</t>
   </si>
@@ -90,13 +90,25 @@
   </si>
   <si>
     <t>… add sole (page) by domain</t>
+  </si>
+  <si>
+    <t>Title + path + top header level + descriptor unigrams</t>
+  </si>
+  <si>
+    <t>Best score: 0.8796</t>
+  </si>
+  <si>
+    <t>Using the following parameters:</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.01, 'hidden_layer_sizes': [70, 70, 70], 'max_iter': 300, 'random_state': 5, 'solver': 'lbfgs'}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -104,8 +116,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -115,6 +132,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -131,11 +154,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q53"/>
+  <dimension ref="A1:Q67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56:E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1495,7 +1520,7 @@
         <v>0.64888599999999996</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>5</v>
       </c>
@@ -1506,7 +1531,7 @@
         <v>0.83510200000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>6</v>
       </c>
@@ -1517,7 +1542,7 @@
         <v>0.78468899999999997</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>7</v>
       </c>
@@ -1528,7 +1553,7 @@
         <v>0.65369699999999997</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>8</v>
       </c>
@@ -1539,7 +1564,7 @@
         <v>0.75460499999999997</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>9</v>
       </c>
@@ -1548,6 +1573,140 @@
       </c>
       <c r="C53">
         <v>0.460729</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B56" s="4"/>
+      <c r="C56" s="4"/>
+      <c r="E56" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>0</v>
+      </c>
+      <c r="C57" t="s">
+        <v>1</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>0</v>
+      </c>
+      <c r="B58" t="s">
+        <v>5</v>
+      </c>
+      <c r="C58">
+        <v>0.61790999999999996</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>1</v>
+      </c>
+      <c r="B59" t="s">
+        <v>6</v>
+      </c>
+      <c r="C59">
+        <v>0.64776100000000003</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>2</v>
+      </c>
+      <c r="B60" t="s">
+        <v>7</v>
+      </c>
+      <c r="C60">
+        <v>0.68258700000000005</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>3</v>
+      </c>
+      <c r="B61" t="s">
+        <v>8</v>
+      </c>
+      <c r="C61">
+        <v>0.78706500000000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>4</v>
+      </c>
+      <c r="B62" t="s">
+        <v>9</v>
+      </c>
+      <c r="C62">
+        <v>0.64776100000000003</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>5</v>
+      </c>
+      <c r="B63" t="s">
+        <v>10</v>
+      </c>
+      <c r="C63">
+        <v>0.86666699999999997</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>6</v>
+      </c>
+      <c r="B64" t="s">
+        <v>2</v>
+      </c>
+      <c r="C64">
+        <v>0.83283600000000002</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>7</v>
+      </c>
+      <c r="B65" t="s">
+        <v>11</v>
+      </c>
+      <c r="C65">
+        <v>0.71243800000000002</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>8</v>
+      </c>
+      <c r="B66" t="s">
+        <v>3</v>
+      </c>
+      <c r="C66">
+        <v>0.82189100000000004</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>9</v>
+      </c>
+      <c r="B67" t="s">
+        <v>4</v>
+      </c>
+      <c r="C67">
+        <v>0.48358200000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
checking in changes for sk
</commit_message>
<xml_diff>
--- a/data/orgs/about/about_model_training_results.xlsx
+++ b/data/orgs/about/about_model_training_results.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="4520" yWindow="2860" windowWidth="28800" windowHeight="17600" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Text based features" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="36">
   <si>
     <t>Name</t>
   </si>
@@ -102,13 +103,46 @@
   </si>
   <si>
     <t>{'alpha': 0.01, 'hidden_layer_sizes': [70, 70, 70], 'max_iter': 300, 'random_state': 5, 'solver': 'lbfgs'}</t>
+  </si>
+  <si>
+    <t>pages_in_domain + is_sole_page</t>
+  </si>
+  <si>
+    <t>pages_in_domain + is_sole_page + add num_words</t>
+  </si>
+  <si>
+    <t>pages_in_domain + is_sole_page + is about</t>
+  </si>
+  <si>
+    <t>Baseline (text based features)</t>
+  </si>
+  <si>
+    <t>Add</t>
+  </si>
+  <si>
+    <t>pages_in_domain + is_sole_page + add num_words + num_sentences</t>
+  </si>
+  <si>
+    <t>pages_in_domain + is_about_ftr + share_of_sentences_ftr</t>
+  </si>
+  <si>
+    <t>pages_in_domain + share_of_sentences_ftr</t>
+  </si>
+  <si>
+    <t>pages_in_domain</t>
+  </si>
+  <si>
+    <t>&lt;-- Has most variables and performs just as well</t>
+  </si>
+  <si>
+    <t>More variables could be helpful in hypergrid search</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -117,12 +151,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Courier New"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -141,6 +194,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -154,13 +213,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,8 +504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56:E58"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="P61" sqref="P61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1576,12 +1640,12 @@
       </c>
     </row>
     <row r="56" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
+      <c r="A56" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B56" s="4"/>
-      <c r="C56" s="4"/>
-      <c r="E56" s="5" t="s">
+      <c r="B56" s="6"/>
+      <c r="C56" s="6"/>
+      <c r="E56" s="7" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1592,7 +1656,7 @@
       <c r="C57" t="s">
         <v>1</v>
       </c>
-      <c r="E57" s="5" t="s">
+      <c r="E57" s="7" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1606,7 +1670,7 @@
       <c r="C58">
         <v>0.61790999999999996</v>
       </c>
-      <c r="E58" s="5" t="s">
+      <c r="E58" s="7" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1708,6 +1772,890 @@
       <c r="C67">
         <v>0.48358200000000001</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="31.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="E1" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="I2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>0.79780099999999998</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4">
+        <v>0.62148800000000004</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4">
+        <v>0.58863799999999999</v>
+      </c>
+      <c r="N4" s="4">
+        <v>0</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P4" s="5">
+        <v>0.62148800000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>0.64840799999999998</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5">
+        <v>0.64840799999999998</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K5">
+        <v>0.64840799999999998</v>
+      </c>
+      <c r="N5" s="4">
+        <v>1</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="P5" s="5">
+        <v>0.64840799999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>0.81373700000000004</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6">
+        <v>0.68228299999999997</v>
+      </c>
+      <c r="I6">
+        <v>2</v>
+      </c>
+      <c r="J6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6">
+        <v>0.64840799999999998</v>
+      </c>
+      <c r="N6" s="4">
+        <v>2</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="P6" s="5">
+        <v>0.68228299999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>0.78984699999999997</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7">
+        <v>0.788852</v>
+      </c>
+      <c r="I7">
+        <v>3</v>
+      </c>
+      <c r="J7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K7">
+        <v>0.78586699999999998</v>
+      </c>
+      <c r="N7" s="4">
+        <v>3</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="P7" s="5">
+        <v>0.78685899999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>0.64840799999999998</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8">
+        <v>0.64840799999999998</v>
+      </c>
+      <c r="I8">
+        <v>4</v>
+      </c>
+      <c r="J8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K8">
+        <v>0.64840799999999998</v>
+      </c>
+      <c r="N8" s="4">
+        <v>4</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="P8" s="5">
+        <v>0.64840799999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>0.86255300000000001</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9">
+        <v>0.86454600000000004</v>
+      </c>
+      <c r="I9">
+        <v>5</v>
+      </c>
+      <c r="J9" t="s">
+        <v>10</v>
+      </c>
+      <c r="K9" s="10">
+        <v>0.728105</v>
+      </c>
+      <c r="N9" s="4">
+        <v>5</v>
+      </c>
+      <c r="O9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="P9" s="5">
+        <v>0.86454299999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>0.81772599999999995</v>
+      </c>
+      <c r="E10">
+        <v>6</v>
+      </c>
+      <c r="F10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <v>0.83865999999999996</v>
+      </c>
+      <c r="I10">
+        <v>6</v>
+      </c>
+      <c r="J10" t="s">
+        <v>2</v>
+      </c>
+      <c r="K10">
+        <v>0.836673</v>
+      </c>
+      <c r="N10" s="4">
+        <v>6</v>
+      </c>
+      <c r="O10" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="P10" s="5">
+        <v>0.83865999999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11">
+        <v>0.70912500000000001</v>
+      </c>
+      <c r="E11">
+        <v>7</v>
+      </c>
+      <c r="F11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11">
+        <v>0.71111500000000005</v>
+      </c>
+      <c r="I11">
+        <v>7</v>
+      </c>
+      <c r="J11" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11">
+        <v>0.66432199999999997</v>
+      </c>
+      <c r="N11" s="4">
+        <v>7</v>
+      </c>
+      <c r="O11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="P11" s="5">
+        <v>0.71111500000000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>0.81574500000000005</v>
+      </c>
+      <c r="E12">
+        <v>8</v>
+      </c>
+      <c r="F12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12">
+        <v>0.81972500000000004</v>
+      </c>
+      <c r="I12">
+        <v>8</v>
+      </c>
+      <c r="J12" t="s">
+        <v>3</v>
+      </c>
+      <c r="K12">
+        <v>0.57268399999999997</v>
+      </c>
+      <c r="N12" s="4">
+        <v>8</v>
+      </c>
+      <c r="O12" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="P12" s="5">
+        <v>0.81872699999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>0.48306399999999999</v>
+      </c>
+      <c r="E13">
+        <v>9</v>
+      </c>
+      <c r="F13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13">
+        <v>0.47519299999999998</v>
+      </c>
+      <c r="I13">
+        <v>9</v>
+      </c>
+      <c r="J13" t="s">
+        <v>4</v>
+      </c>
+      <c r="K13">
+        <v>0.49417899999999998</v>
+      </c>
+      <c r="N13" s="4">
+        <v>9</v>
+      </c>
+      <c r="O13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="P13" s="5">
+        <v>0.496091</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="N16" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+    </row>
+    <row r="17" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="O17" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="P17" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18">
+        <v>0.60560099999999994</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18">
+        <v>0.80577399999999999</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18" t="s">
+        <v>5</v>
+      </c>
+      <c r="K18">
+        <v>0.80179</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18" t="s">
+        <v>5</v>
+      </c>
+      <c r="P18">
+        <v>0.80179</v>
+      </c>
+      <c r="R18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19">
+        <v>0.64840799999999998</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19">
+        <v>0.64840799999999998</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19" t="s">
+        <v>6</v>
+      </c>
+      <c r="K19">
+        <v>0.64940299999999995</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
+      <c r="O19" t="s">
+        <v>6</v>
+      </c>
+      <c r="P19">
+        <v>0.64940299999999995</v>
+      </c>
+      <c r="R19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20">
+        <v>0.64940600000000004</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+      <c r="F20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20">
+        <v>0.81971300000000002</v>
+      </c>
+      <c r="I20">
+        <v>2</v>
+      </c>
+      <c r="J20" t="s">
+        <v>7</v>
+      </c>
+      <c r="K20">
+        <v>0.81970699999999996</v>
+      </c>
+      <c r="N20">
+        <v>2</v>
+      </c>
+      <c r="O20" t="s">
+        <v>7</v>
+      </c>
+      <c r="P20">
+        <v>0.81970699999999996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>3</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21">
+        <v>0.78785700000000003</v>
+      </c>
+      <c r="E21">
+        <v>3</v>
+      </c>
+      <c r="F21" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21">
+        <v>0.788852</v>
+      </c>
+      <c r="I21">
+        <v>3</v>
+      </c>
+      <c r="J21" t="s">
+        <v>8</v>
+      </c>
+      <c r="K21">
+        <v>0.78785700000000003</v>
+      </c>
+      <c r="N21">
+        <v>3</v>
+      </c>
+      <c r="O21" t="s">
+        <v>8</v>
+      </c>
+      <c r="P21">
+        <v>0.78785700000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>4</v>
+      </c>
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22">
+        <v>0.64840799999999998</v>
+      </c>
+      <c r="E22">
+        <v>4</v>
+      </c>
+      <c r="F22" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22">
+        <v>0.64840799999999998</v>
+      </c>
+      <c r="I22">
+        <v>4</v>
+      </c>
+      <c r="J22" t="s">
+        <v>9</v>
+      </c>
+      <c r="K22">
+        <v>0.64840799999999998</v>
+      </c>
+      <c r="N22">
+        <v>4</v>
+      </c>
+      <c r="O22" t="s">
+        <v>9</v>
+      </c>
+      <c r="P22">
+        <v>0.64840799999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>5</v>
+      </c>
+      <c r="B23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23">
+        <v>0.85757399999999995</v>
+      </c>
+      <c r="E23">
+        <v>5</v>
+      </c>
+      <c r="F23" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23">
+        <v>0.86353599999999997</v>
+      </c>
+      <c r="I23">
+        <v>5</v>
+      </c>
+      <c r="J23" t="s">
+        <v>10</v>
+      </c>
+      <c r="K23">
+        <v>0.862541</v>
+      </c>
+      <c r="N23">
+        <v>5</v>
+      </c>
+      <c r="O23" t="s">
+        <v>10</v>
+      </c>
+      <c r="P23">
+        <v>0.86453100000000005</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>6</v>
+      </c>
+      <c r="B24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>0.83564499999999997</v>
+      </c>
+      <c r="E24">
+        <v>6</v>
+      </c>
+      <c r="F24" t="s">
+        <v>2</v>
+      </c>
+      <c r="G24">
+        <v>0.83865999999999996</v>
+      </c>
+      <c r="I24">
+        <v>6</v>
+      </c>
+      <c r="J24" t="s">
+        <v>2</v>
+      </c>
+      <c r="K24">
+        <v>0.82869499999999996</v>
+      </c>
+      <c r="N24">
+        <v>6</v>
+      </c>
+      <c r="O24" t="s">
+        <v>2</v>
+      </c>
+      <c r="P24">
+        <v>0.82869499999999996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>7</v>
+      </c>
+      <c r="B25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25">
+        <v>0.71111500000000005</v>
+      </c>
+      <c r="E25">
+        <v>7</v>
+      </c>
+      <c r="F25" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25">
+        <v>0.70912500000000001</v>
+      </c>
+      <c r="I25">
+        <v>7</v>
+      </c>
+      <c r="J25" t="s">
+        <v>11</v>
+      </c>
+      <c r="K25">
+        <v>0.70912500000000001</v>
+      </c>
+      <c r="N25">
+        <v>7</v>
+      </c>
+      <c r="O25" t="s">
+        <v>11</v>
+      </c>
+      <c r="P25">
+        <v>0.70912500000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>8</v>
+      </c>
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26">
+        <v>0.78088299999999999</v>
+      </c>
+      <c r="E26">
+        <v>8</v>
+      </c>
+      <c r="F26" t="s">
+        <v>3</v>
+      </c>
+      <c r="G26">
+        <v>0.83267800000000003</v>
+      </c>
+      <c r="I26">
+        <v>8</v>
+      </c>
+      <c r="J26" t="s">
+        <v>3</v>
+      </c>
+      <c r="K26">
+        <v>0.83666399999999996</v>
+      </c>
+      <c r="N26">
+        <v>8</v>
+      </c>
+      <c r="O26" t="s">
+        <v>3</v>
+      </c>
+      <c r="P26">
+        <v>0.83666399999999996</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>9</v>
+      </c>
+      <c r="B27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27">
+        <v>0.56481700000000001</v>
+      </c>
+      <c r="E27">
+        <v>9</v>
+      </c>
+      <c r="F27" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27">
+        <v>0.48601</v>
+      </c>
+      <c r="I27">
+        <v>9</v>
+      </c>
+      <c r="J27" t="s">
+        <v>4</v>
+      </c>
+      <c r="K27">
+        <v>0.522895</v>
+      </c>
+      <c r="N27">
+        <v>9</v>
+      </c>
+      <c r="O27" t="s">
+        <v>4</v>
+      </c>
+      <c r="P27">
+        <v>0.522895</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" ht="19" x14ac:dyDescent="0.25">
+      <c r="B30" s="7"/>
+    </row>
+    <row r="31" spans="1:18" ht="19" x14ac:dyDescent="0.25">
+      <c r="B31" s="7"/>
+    </row>
+    <row r="32" spans="1:18" ht="19" x14ac:dyDescent="0.25">
+      <c r="B32" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add home pages after prediction model
</commit_message>
<xml_diff>
--- a/data/orgs/about/about_model_training_results.xlsx
+++ b/data/orgs/about/about_model_training_results.xlsx
@@ -9,11 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4520" yWindow="2860" windowWidth="28800" windowHeight="17600" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1740" yWindow="1820" windowWidth="31400" windowHeight="18920" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Text based features" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Count based features" sheetId="2" r:id="rId2"/>
+    <sheet name="Final" sheetId="3" r:id="rId3"/>
+    <sheet name="Final_T" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="40">
   <si>
     <t>Name</t>
   </si>
@@ -137,12 +139,35 @@
   <si>
     <t>More variables could be helpful in hypergrid search</t>
   </si>
+  <si>
+    <t>All features</t>
+  </si>
+  <si>
+    <t>Text features</t>
+  </si>
+  <si>
+    <t>Count based features</t>
+  </si>
+  <si>
+    <t>All features minus header text</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="8" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -173,6 +198,22 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Courier New"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -210,23 +251,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -237,6 +285,2519 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Final!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Count based features</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Final!$A$2:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Nearest Neighbors</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Linear SVM</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>RBF SVM</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Decision Tree</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Random Forest</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Neural Net</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>AdaBoost</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Naive Bayes</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>SVC</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>QDA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Final!$B$2:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.000_);_(* \(#,##0.000\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.672622</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.732463</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.72696</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.741406</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.744155</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.737275</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.735209</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.739339</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.691883</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.732463</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Final!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Text features</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Final!$A$2:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Nearest Neighbors</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Linear SVM</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>RBF SVM</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Decision Tree</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Random Forest</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Neural Net</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>AdaBoost</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Naive Bayes</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>SVC</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>QDA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Final!$C$2:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.000_);_(* \(#,##0.000\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.81843</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.732463</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.831496</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.814322</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.732463</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.875515</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.843184</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.727604</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.831506</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.344597</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Final!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>All features minus header text</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Final!$A$2:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Nearest Neighbors</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Linear SVM</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>RBF SVM</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Decision Tree</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Random Forest</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Neural Net</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>AdaBoost</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Naive Bayes</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>SVC</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>QDA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Final!$D$2:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.000_);_(* \(#,##0.000\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.825306</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.732463</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.828747</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.804675</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.732463</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.887216</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.86521</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.728984</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.841142</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.482869</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Final!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>All features</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Final!$A$2:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Nearest Neighbors</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Linear SVM</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>RBF SVM</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Decision Tree</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Random Forest</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Neural Net</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>AdaBoost</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Naive Bayes</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>SVC</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>QDA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Final!$E$2:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.000_);_(* \(#,##0.000\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.821864</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.732463</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.83287</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.815008</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.732463</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.892034</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.851447</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.729668</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.847329</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.456059</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1129731040"/>
+        <c:axId val="1796017312"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1129731040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1796017312"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1796017312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1129731040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Final_T!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Count based features</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Final_T!$B$1:$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Nearest Neighbors</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Linear SVM</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>RBF SVM</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Decision Tree</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Random Forest</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Neural Net</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>AdaBoost</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Naive Bayes</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>SVC</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>QDA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Final_T!$B$2:$K$2</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.000_);_(* \(#,##0.000\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.672622</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.732463</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.72696</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.741406</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.744155</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.737275</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.735209</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.739339</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.691883</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.732463</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Final_T!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Text features</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Final_T!$B$1:$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Nearest Neighbors</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Linear SVM</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>RBF SVM</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Decision Tree</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Random Forest</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Neural Net</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>AdaBoost</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Naive Bayes</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>SVC</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>QDA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Final_T!$B$3:$K$3</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.000_);_(* \(#,##0.000\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.81843</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.732463</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.831496</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.814322</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.732463</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.875515</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.843184</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.727604</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.831506</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.344597</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Final_T!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>All features minus header text</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Final_T!$B$1:$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Nearest Neighbors</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Linear SVM</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>RBF SVM</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Decision Tree</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Random Forest</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Neural Net</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>AdaBoost</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Naive Bayes</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>SVC</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>QDA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Final_T!$B$4:$K$4</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.000_);_(* \(#,##0.000\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.825306</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.732463</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.828747</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.804675</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.732463</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.887216</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.86521</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.728984</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.841142</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.482869</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Final_T!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>All features</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Final_T!$B$1:$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Nearest Neighbors</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Linear SVM</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>RBF SVM</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Decision Tree</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Random Forest</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Neural Net</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>AdaBoost</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Naive Bayes</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>SVC</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>QDA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Final_T!$B$5:$K$5</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.000_);_(* \(#,##0.000\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.821864</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.732463</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.83287</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.815008</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.732463</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.892034</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.851447</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.729668</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.847329</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.456059</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1221887728"/>
+        <c:axId val="1106627152"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1221887728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1106627152"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1106627152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1221887728"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>626534</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>118534</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>16932</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1782,7 +4343,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
@@ -2660,4 +5221,407 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.1640625" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="11">
+        <v>0.67262200000000005</v>
+      </c>
+      <c r="C2" s="11">
+        <v>0.81842999999999999</v>
+      </c>
+      <c r="D2" s="11">
+        <v>0.82530599999999998</v>
+      </c>
+      <c r="E2" s="11">
+        <v>0.82186400000000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="11">
+        <v>0.73246299999999998</v>
+      </c>
+      <c r="C3" s="11">
+        <v>0.73246299999999998</v>
+      </c>
+      <c r="D3" s="11">
+        <v>0.73246299999999998</v>
+      </c>
+      <c r="E3" s="11">
+        <v>0.73246299999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="11">
+        <v>0.72696000000000005</v>
+      </c>
+      <c r="C4" s="11">
+        <v>0.83149600000000001</v>
+      </c>
+      <c r="D4" s="11">
+        <v>0.82874700000000001</v>
+      </c>
+      <c r="E4" s="11">
+        <v>0.83287</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="11">
+        <v>0.74140600000000001</v>
+      </c>
+      <c r="C5" s="11">
+        <v>0.81432199999999999</v>
+      </c>
+      <c r="D5" s="11">
+        <v>0.80467500000000003</v>
+      </c>
+      <c r="E5" s="11">
+        <v>0.81500799999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="11">
+        <v>0.74415500000000001</v>
+      </c>
+      <c r="C6" s="11">
+        <v>0.73246299999999998</v>
+      </c>
+      <c r="D6" s="11">
+        <v>0.73246299999999998</v>
+      </c>
+      <c r="E6" s="11">
+        <v>0.73246299999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="11">
+        <v>0.73727500000000001</v>
+      </c>
+      <c r="C7" s="11">
+        <v>0.87551500000000004</v>
+      </c>
+      <c r="D7" s="11">
+        <v>0.887216</v>
+      </c>
+      <c r="E7" s="11">
+        <v>0.89203399999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="11">
+        <v>0.735209</v>
+      </c>
+      <c r="C8" s="11">
+        <v>0.84318400000000004</v>
+      </c>
+      <c r="D8" s="11">
+        <v>0.86521000000000003</v>
+      </c>
+      <c r="E8" s="11">
+        <v>0.85144699999999995</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="11">
+        <v>0.73933899999999997</v>
+      </c>
+      <c r="C9" s="11">
+        <v>0.72760400000000003</v>
+      </c>
+      <c r="D9" s="11">
+        <v>0.72898399999999997</v>
+      </c>
+      <c r="E9" s="11">
+        <v>0.72966799999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="11">
+        <v>0.69188300000000003</v>
+      </c>
+      <c r="C10" s="11">
+        <v>0.83150599999999997</v>
+      </c>
+      <c r="D10" s="11">
+        <v>0.84114199999999995</v>
+      </c>
+      <c r="E10" s="11">
+        <v>0.847329</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="11">
+        <v>0.73246299999999998</v>
+      </c>
+      <c r="C11" s="11">
+        <v>0.34459699999999999</v>
+      </c>
+      <c r="D11" s="11">
+        <v>0.48286899999999999</v>
+      </c>
+      <c r="E11" s="11">
+        <v>0.45605899999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="11">
+        <v>0.67262200000000005</v>
+      </c>
+      <c r="C2" s="11">
+        <v>0.73246299999999998</v>
+      </c>
+      <c r="D2" s="11">
+        <v>0.72696000000000005</v>
+      </c>
+      <c r="E2" s="11">
+        <v>0.74140600000000001</v>
+      </c>
+      <c r="F2" s="11">
+        <v>0.74415500000000001</v>
+      </c>
+      <c r="G2" s="11">
+        <v>0.73727500000000001</v>
+      </c>
+      <c r="H2" s="11">
+        <v>0.735209</v>
+      </c>
+      <c r="I2" s="11">
+        <v>0.73933899999999997</v>
+      </c>
+      <c r="J2" s="11">
+        <v>0.69188300000000003</v>
+      </c>
+      <c r="K2" s="11">
+        <v>0.73246299999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="11">
+        <v>0.81842999999999999</v>
+      </c>
+      <c r="C3" s="11">
+        <v>0.73246299999999998</v>
+      </c>
+      <c r="D3" s="11">
+        <v>0.83149600000000001</v>
+      </c>
+      <c r="E3" s="11">
+        <v>0.81432199999999999</v>
+      </c>
+      <c r="F3" s="11">
+        <v>0.73246299999999998</v>
+      </c>
+      <c r="G3" s="11">
+        <v>0.87551500000000004</v>
+      </c>
+      <c r="H3" s="11">
+        <v>0.84318400000000004</v>
+      </c>
+      <c r="I3" s="11">
+        <v>0.72760400000000003</v>
+      </c>
+      <c r="J3" s="11">
+        <v>0.83150599999999997</v>
+      </c>
+      <c r="K3" s="11">
+        <v>0.34459699999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="11">
+        <v>0.82530599999999998</v>
+      </c>
+      <c r="C4" s="11">
+        <v>0.73246299999999998</v>
+      </c>
+      <c r="D4" s="11">
+        <v>0.82874700000000001</v>
+      </c>
+      <c r="E4" s="11">
+        <v>0.80467500000000003</v>
+      </c>
+      <c r="F4" s="11">
+        <v>0.73246299999999998</v>
+      </c>
+      <c r="G4" s="11">
+        <v>0.887216</v>
+      </c>
+      <c r="H4" s="11">
+        <v>0.86521000000000003</v>
+      </c>
+      <c r="I4" s="11">
+        <v>0.72898399999999997</v>
+      </c>
+      <c r="J4" s="11">
+        <v>0.84114199999999995</v>
+      </c>
+      <c r="K4" s="11">
+        <v>0.48286899999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="11">
+        <v>0.82186400000000004</v>
+      </c>
+      <c r="C5" s="11">
+        <v>0.73246299999999998</v>
+      </c>
+      <c r="D5" s="11">
+        <v>0.83287</v>
+      </c>
+      <c r="E5" s="11">
+        <v>0.81500799999999995</v>
+      </c>
+      <c r="F5" s="11">
+        <v>0.73246299999999998</v>
+      </c>
+      <c r="G5" s="11">
+        <v>0.89203399999999999</v>
+      </c>
+      <c r="H5" s="11">
+        <v>0.85144699999999995</v>
+      </c>
+      <c r="I5" s="11">
+        <v>0.72966799999999998</v>
+      </c>
+      <c r="J5" s="11">
+        <v>0.847329</v>
+      </c>
+      <c r="K5" s="11">
+        <v>0.45605899999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>